<commit_message>
Modificacion sobre acciones correctivas
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-150430.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-150430.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Acciones correctivas</t>
   </si>
@@ -58,10 +58,22 @@
     <t>Jovanny zepeda</t>
   </si>
   <si>
-    <t>Se omite un respaldo de uan semana</t>
-  </si>
-  <si>
     <t>Se genera respado la semana entrante</t>
+  </si>
+  <si>
+    <t>Se omite un respaldo de una semana</t>
+  </si>
+  <si>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Por omicion a la generacion de encuestas de satisfaccion existen resultados invalidos en la seccion de satisfaccion</t>
+  </si>
+  <si>
+    <t>Generar lo mas pronto posible las encuestas de satisfaccion</t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
   </si>
 </sst>
 </file>
@@ -194,11 +206,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -521,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -544,30 +556,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C4" s="9" t="s">
@@ -599,7 +611,7 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -615,27 +627,27 @@
         <v>42094</v>
       </c>
       <c r="I5" s="7">
-        <v>42094</v>
+        <v>42124</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="11">
         <v>2</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F6" s="5">
         <v>42094</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H6" s="7">
         <v>42124</v>
@@ -647,13 +659,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="C7" s="1"/>
-      <c r="D7" s="13" t="s">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="C7" s="11">
+        <v>3</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="F7" s="7">
         <v>42124</v>
@@ -664,22 +678,20 @@
       <c r="H7" s="7">
         <v>42144</v>
       </c>
-      <c r="I7" s="7">
-        <v>42144</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
@@ -811,15 +823,15 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
@@ -862,13 +874,13 @@
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="3:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="3:10" ht="15" x14ac:dyDescent="0.25">
@@ -880,6 +892,16 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="3:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -896,10 +918,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28">
-      <formula1>$L$5:$L$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J29">
+      <formula1>$L$5:$L$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J28">
       <formula1>"Abierto, Proceso, Cerrado, Cancelado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>